<commit_message>
percent changes fix' '
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,12 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="1">
   <si>
-    <t xml:space="preserve">test2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test2</t>
+    <t xml:space="preserve">test</t>
   </si>
 </sst>
 </file>
@@ -124,44 +121,174 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A2:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.3214285714286"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1991</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1992</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1993</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1993</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1993</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1993</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1993</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1993</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>